<commit_message>
subida agenda de materia
</commit_message>
<xml_diff>
--- a/Documentos/Agenda_alumnos.xlsx
+++ b/Documentos/Agenda_alumnos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\electiva-1-2015\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\electiva-programacion-1-2015\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -364,16 +364,16 @@
     <t>https://code.google.com/p/electiva-de-programacion-nur-2-2014/</t>
   </si>
   <si>
-    <t>URL del repositorio en Bitbucket</t>
-  </si>
-  <si>
-    <t>https://bitbucket.org/jmacboy/electiva-de-programacion-1-2015</t>
-  </si>
-  <si>
     <t>https://www.dropbox.com/sh/lwm16uwdz2vsn49/AADQYTjcVM88LjvKGucEmOQ0a?dl=0</t>
   </si>
   <si>
     <t>Alicia Palacios</t>
+  </si>
+  <si>
+    <t>URL del repositorio en Github</t>
+  </si>
+  <si>
+    <t>https://github.com/jmacboy/electiva-programacion-1-2015/tree/master/Documentos</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1622,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.35">
@@ -1750,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1994,7 +1994,7 @@
   <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.7" x14ac:dyDescent="0.25"/>
@@ -2034,17 +2034,17 @@
         <v>34</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -2111,10 +2111,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
subida direccion de videos
</commit_message>
<xml_diff>
--- a/Documentos/Agenda_alumnos.xlsx
+++ b/Documentos/Agenda_alumnos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Fecha</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>https://github.com/jmacboy/electiva-programacion-1-2015/tree/master</t>
+  </si>
+  <si>
+    <t>URL de Videos</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/sh/h09pcu3qlixke56/AABwbfOIUiDE73HA5oko10iCa?dl=0</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2000,7 @@
   <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.7" x14ac:dyDescent="0.25"/>
@@ -2049,8 +2055,12 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.35">
-      <c r="B7" s="6"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
@@ -2112,9 +2122,10 @@
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
subidas todas las prácticas
</commit_message>
<xml_diff>
--- a/Documentos/Agenda_alumnos.xlsx
+++ b/Documentos/Agenda_alumnos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="357" yWindow="104" windowWidth="9181" windowHeight="4274" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="357" yWindow="104" windowWidth="9181" windowHeight="4274" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>Fecha</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>https://www.dropbox.com/sh/h09pcu3qlixke56/AABwbfOIUiDE73HA5oko10iCa?dl=0</t>
+  </si>
+  <si>
+    <t>Abel Claure</t>
   </si>
 </sst>
 </file>
@@ -1568,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.7" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1686,9 @@
       <c r="C12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="40" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.55" x14ac:dyDescent="0.25">
       <c r="B13" s="43" t="s">
@@ -1999,7 +2004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>